<commit_message>
Eksport  import transaksi penjualan
</commit_message>
<xml_diff>
--- a/POS/public/template_penjualan.xlsx
+++ b/POS/public/template_penjualan.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_2025\POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0923AFBB-A1AB-47D5-A432-4907D804054E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD773A7C-9AE6-4B8F-AEC1-AACE28C3A973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{EABFBDEB-C3A8-42E3-A0BE-23E547DA520B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A7E97B80-A418-492F-A732-970E08D29917}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>user_id</t>
   </si>
@@ -45,39 +45,41 @@
     <t>pembeli</t>
   </si>
   <si>
-    <t>penjualan_tanggal</t>
-  </si>
-  <si>
-    <t>TRX0012</t>
-  </si>
-  <si>
-    <t>TRX0011</t>
-  </si>
-  <si>
-    <t>TRX0013</t>
-  </si>
-  <si>
-    <t>Customer 11</t>
-  </si>
-  <si>
-    <t>Customer 12</t>
-  </si>
-  <si>
-    <t>Customer 13</t>
+    <t>barang_id</t>
+  </si>
+  <si>
+    <t>jumlah</t>
+  </si>
+  <si>
+    <t>TXR0015</t>
+  </si>
+  <si>
+    <t>Customer 15</t>
+  </si>
+  <si>
+    <t>Customer 16</t>
+  </si>
+  <si>
+    <t>TXR0016</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-  </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -102,9 +104,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -133,39 +138,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -217,7 +222,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -328,13 +333,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -343,6 +341,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -407,47 +412,69 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{414A7F9B-A861-4031-856B-D5C837052CA6}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE8EE6D-4B72-42E2-BFD1-A7CC2131E7D3}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.90625" customWidth="1"/>
-    <col min="4" max="4" width="20.453125" customWidth="1"/>
+    <col min="2" max="2" width="20.26953125" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" customWidth="1"/>
+    <col min="4" max="4" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>3</v>
       </c>
@@ -455,41 +482,38 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="str">
-        <f ca="1">TEXT(NOW(), "yyyy-mm-dd_hh:mm:ss")</f>
-        <v>2025-04-12 21:09:01</v>
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="str">
-        <f t="shared" ref="D3:D4" ca="1" si="0">TEXT(NOW(), "yyyy-mm-dd_hh:mm:ss")</f>
-        <v>2025-04-12 21:09:01</v>
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="1" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>2025-04-12 21:09:01</v>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D4">
+        <v>28</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Coba import data penjualan
</commit_message>
<xml_diff>
--- a/POS/public/template_penjualan.xlsx
+++ b/POS/public/template_penjualan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_2025\POS\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aqila Nur\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD773A7C-9AE6-4B8F-AEC1-AACE28C3A973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6354EF68-DFD9-4FDA-9E2B-517C528CCFAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A7E97B80-A418-492F-A732-970E08D29917}"/>
   </bookViews>
@@ -51,16 +51,16 @@
     <t>jumlah</t>
   </si>
   <si>
-    <t>TXR0015</t>
-  </si>
-  <si>
-    <t>Customer 15</t>
-  </si>
-  <si>
-    <t>Customer 16</t>
-  </si>
-  <si>
-    <t>TXR0016</t>
+    <t>TXR0022</t>
+  </si>
+  <si>
+    <t>TXR0023</t>
+  </si>
+  <si>
+    <t>Customer 22</t>
+  </si>
+  <si>
+    <t>Customer 23</t>
   </si>
 </sst>
 </file>
@@ -447,7 +447,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -482,10 +482,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -496,13 +496,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
       <c r="D3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>1</v>

</xml_diff>